<commit_message>
Git007 -updated september month expenses
</commit_message>
<xml_diff>
--- a/TestMonthlyExpense/src/main/resources/HouseExpenseChart.xlsx
+++ b/TestMonthlyExpense/src/main/resources/HouseExpenseChart.xlsx
@@ -4,17 +4,18 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="August" sheetId="2" r:id="rId1"/>
+    <sheet name="September" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="442" uniqueCount="149">
   <si>
     <t>GF</t>
   </si>
@@ -362,6 +363,105 @@
   </si>
   <si>
     <t>MS</t>
+  </si>
+  <si>
+    <t>Noodles 560g</t>
+  </si>
+  <si>
+    <t>Harpic cit</t>
+  </si>
+  <si>
+    <t>Harpic pow</t>
+  </si>
+  <si>
+    <t>Lizol lav</t>
+  </si>
+  <si>
+    <t>Lizol cit</t>
+  </si>
+  <si>
+    <t>Dish wash Liquid 500ml</t>
+  </si>
+  <si>
+    <t>Black Mookadalai 1kg</t>
+  </si>
+  <si>
+    <t>Twinkle</t>
+  </si>
+  <si>
+    <t>Scrubber pad</t>
+  </si>
+  <si>
+    <t>Bath Soap 75g</t>
+  </si>
+  <si>
+    <t>Semiya 900g</t>
+  </si>
+  <si>
+    <t>Surf excel</t>
+  </si>
+  <si>
+    <t>Yardly</t>
+  </si>
+  <si>
+    <t>Body Deodarant</t>
+  </si>
+  <si>
+    <t>Hamam</t>
+  </si>
+  <si>
+    <t>Samba Ravai 500g</t>
+  </si>
+  <si>
+    <t>Cashewnut 200g</t>
+  </si>
+  <si>
+    <t>Cumin seeds 200g</t>
+  </si>
+  <si>
+    <t>Pepper 200g</t>
+  </si>
+  <si>
+    <t>Mustard 200g</t>
+  </si>
+  <si>
+    <t>Green Moong dhal</t>
+  </si>
+  <si>
+    <t>Aval 500g</t>
+  </si>
+  <si>
+    <t>Raisins 500g</t>
+  </si>
+  <si>
+    <t>Green peas 200g</t>
+  </si>
+  <si>
+    <t>Poppy 50g</t>
+  </si>
+  <si>
+    <t>Methi 200g</t>
+  </si>
+  <si>
+    <t>Cardamom 25g</t>
+  </si>
+  <si>
+    <t>Roasted Rava 1kg</t>
+  </si>
+  <si>
+    <t>Pepsodent</t>
+  </si>
+  <si>
+    <t>Toothpaste 80g</t>
+  </si>
+  <si>
+    <t>Kalpasi 10g</t>
+  </si>
+  <si>
+    <t>Aacturm powder 100g</t>
+  </si>
+  <si>
+    <t>September</t>
   </si>
 </sst>
 </file>
@@ -1244,8 +1344,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2712,4 +2812,1179 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G48"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3:G48"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="3">
+        <v>239</v>
+      </c>
+      <c r="D2" s="3">
+        <v>4</v>
+      </c>
+      <c r="E2" s="3">
+        <f>C2*D2</f>
+        <v>956</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="C3" s="3">
+        <v>71</v>
+      </c>
+      <c r="D3" s="3">
+        <v>1</v>
+      </c>
+      <c r="E3" s="3">
+        <f t="shared" ref="E3:E30" si="0">C3*D3</f>
+        <v>71</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="C4" s="3">
+        <v>54.5</v>
+      </c>
+      <c r="D4" s="3">
+        <v>1</v>
+      </c>
+      <c r="E4" s="3">
+        <f t="shared" si="0"/>
+        <v>54.5</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="3">
+        <v>200.5</v>
+      </c>
+      <c r="D5" s="3">
+        <v>1</v>
+      </c>
+      <c r="E5" s="3">
+        <f t="shared" si="0"/>
+        <v>200.5</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C6" s="3">
+        <v>226</v>
+      </c>
+      <c r="D6" s="3">
+        <v>2</v>
+      </c>
+      <c r="E6" s="3">
+        <f t="shared" si="0"/>
+        <v>452</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="3">
+        <v>66</v>
+      </c>
+      <c r="D7" s="3">
+        <v>2</v>
+      </c>
+      <c r="E7" s="3">
+        <f t="shared" ref="E7" si="1">C7*D7</f>
+        <v>132</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="3">
+        <v>65</v>
+      </c>
+      <c r="D8" s="3">
+        <v>2</v>
+      </c>
+      <c r="E8" s="3">
+        <f t="shared" si="0"/>
+        <v>130</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="3">
+        <v>64</v>
+      </c>
+      <c r="D9" s="3">
+        <v>1</v>
+      </c>
+      <c r="E9" s="3">
+        <f t="shared" si="0"/>
+        <v>64</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="3">
+        <v>65</v>
+      </c>
+      <c r="D10" s="3">
+        <v>1</v>
+      </c>
+      <c r="E10" s="3">
+        <f t="shared" ref="E10" si="2">C10*D10</f>
+        <v>65</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="C11" s="3">
+        <v>88</v>
+      </c>
+      <c r="D11" s="3">
+        <v>1</v>
+      </c>
+      <c r="E11" s="3">
+        <f t="shared" si="0"/>
+        <v>88</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" s="3">
+        <v>79</v>
+      </c>
+      <c r="D12" s="3">
+        <v>1</v>
+      </c>
+      <c r="E12" s="3">
+        <f t="shared" si="0"/>
+        <v>79</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13" s="3">
+        <v>22.5</v>
+      </c>
+      <c r="D13" s="3">
+        <v>1</v>
+      </c>
+      <c r="E13" s="3">
+        <f t="shared" si="0"/>
+        <v>22.5</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14" s="3">
+        <v>41</v>
+      </c>
+      <c r="D14" s="3">
+        <v>1</v>
+      </c>
+      <c r="E14" s="3">
+        <f t="shared" si="0"/>
+        <v>41</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C15" s="3">
+        <v>128</v>
+      </c>
+      <c r="D15" s="3">
+        <v>2</v>
+      </c>
+      <c r="E15" s="3">
+        <f t="shared" si="0"/>
+        <v>256</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C16" s="3">
+        <v>18</v>
+      </c>
+      <c r="D16" s="3">
+        <v>1</v>
+      </c>
+      <c r="E16" s="3">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C17" s="3">
+        <v>85</v>
+      </c>
+      <c r="D17" s="3">
+        <v>1</v>
+      </c>
+      <c r="E17" s="3">
+        <f t="shared" si="0"/>
+        <v>85</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="C18" s="3">
+        <v>77</v>
+      </c>
+      <c r="D18" s="3">
+        <v>1</v>
+      </c>
+      <c r="E18" s="3">
+        <f t="shared" si="0"/>
+        <v>77</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C19" s="3">
+        <v>8</v>
+      </c>
+      <c r="D19" s="3">
+        <v>1</v>
+      </c>
+      <c r="E19" s="3">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C20" s="3">
+        <v>240.5</v>
+      </c>
+      <c r="D20" s="3">
+        <v>1</v>
+      </c>
+      <c r="E20" s="3">
+        <f t="shared" si="0"/>
+        <v>240.5</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C21" s="3">
+        <v>48.5</v>
+      </c>
+      <c r="D21" s="3">
+        <v>1</v>
+      </c>
+      <c r="E21" s="3">
+        <f t="shared" si="0"/>
+        <v>48.5</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G21" s="3" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="C22" s="3">
+        <v>9.5</v>
+      </c>
+      <c r="D22" s="3">
+        <v>3</v>
+      </c>
+      <c r="E22" s="3">
+        <f t="shared" si="0"/>
+        <v>28.5</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C23" s="3">
+        <v>14</v>
+      </c>
+      <c r="D23" s="3">
+        <v>2</v>
+      </c>
+      <c r="E23" s="3">
+        <f t="shared" ref="E23" si="3">C23*D23</f>
+        <v>28</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G23" s="3" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C24" s="3">
+        <v>72.5</v>
+      </c>
+      <c r="D24" s="3">
+        <v>1</v>
+      </c>
+      <c r="E24" s="3">
+        <f t="shared" si="0"/>
+        <v>72.5</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="G24" s="3" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="C25" s="3">
+        <v>43.5</v>
+      </c>
+      <c r="D25" s="3">
+        <v>1</v>
+      </c>
+      <c r="E25" s="3">
+        <f t="shared" si="0"/>
+        <v>43.5</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G25" s="3" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C26" s="3">
+        <v>20</v>
+      </c>
+      <c r="D26" s="3">
+        <v>1</v>
+      </c>
+      <c r="E26" s="3">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G26" s="3" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C27" s="3">
+        <v>105</v>
+      </c>
+      <c r="D27" s="3">
+        <v>1</v>
+      </c>
+      <c r="E27" s="3">
+        <f t="shared" si="0"/>
+        <v>105</v>
+      </c>
+      <c r="F27" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G27" s="3" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C28" s="3">
+        <v>132</v>
+      </c>
+      <c r="D28" s="3">
+        <v>1</v>
+      </c>
+      <c r="E28" s="3">
+        <f t="shared" si="0"/>
+        <v>132</v>
+      </c>
+      <c r="F28" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G28" s="3" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="C29" s="3">
+        <v>59.5</v>
+      </c>
+      <c r="D29" s="3">
+        <v>1</v>
+      </c>
+      <c r="E29" s="3">
+        <f t="shared" si="0"/>
+        <v>59.5</v>
+      </c>
+      <c r="F29" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G29" s="3" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="C30" s="3">
+        <v>150</v>
+      </c>
+      <c r="D30" s="3">
+        <v>1</v>
+      </c>
+      <c r="E30" s="3">
+        <f t="shared" si="0"/>
+        <v>150</v>
+      </c>
+      <c r="F30" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G30" s="3" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="C31" s="3">
+        <v>178</v>
+      </c>
+      <c r="D31" s="3">
+        <v>1</v>
+      </c>
+      <c r="E31" s="3">
+        <f t="shared" ref="E31:E46" si="4">C31*D31</f>
+        <v>178</v>
+      </c>
+      <c r="F31" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G31" s="3" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C32" s="3">
+        <v>25</v>
+      </c>
+      <c r="D32" s="3">
+        <v>4</v>
+      </c>
+      <c r="E32" s="3">
+        <f t="shared" si="4"/>
+        <v>100</v>
+      </c>
+      <c r="F32" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G32" s="3" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="C33" s="3">
+        <v>50</v>
+      </c>
+      <c r="D33" s="3">
+        <v>1</v>
+      </c>
+      <c r="E33" s="3">
+        <f t="shared" si="4"/>
+        <v>50</v>
+      </c>
+      <c r="F33" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G33" s="3" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="C34" s="3">
+        <v>180</v>
+      </c>
+      <c r="D34" s="3">
+        <v>1</v>
+      </c>
+      <c r="E34" s="3">
+        <f t="shared" si="4"/>
+        <v>180</v>
+      </c>
+      <c r="F34" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G34" s="3" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="C35" s="3">
+        <v>50</v>
+      </c>
+      <c r="D35" s="3">
+        <v>1</v>
+      </c>
+      <c r="E35" s="3">
+        <f t="shared" si="4"/>
+        <v>50</v>
+      </c>
+      <c r="F35" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G35" s="3" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="C36" s="3">
+        <v>216</v>
+      </c>
+      <c r="D36" s="3">
+        <v>1</v>
+      </c>
+      <c r="E36" s="3">
+        <f t="shared" si="4"/>
+        <v>216</v>
+      </c>
+      <c r="F36" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G36" s="3" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="C37" s="3">
+        <v>20</v>
+      </c>
+      <c r="D37" s="3">
+        <v>2</v>
+      </c>
+      <c r="E37" s="3">
+        <f t="shared" si="4"/>
+        <v>40</v>
+      </c>
+      <c r="F37" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G37" s="3" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="C38" s="3">
+        <v>57</v>
+      </c>
+      <c r="D38" s="3">
+        <v>1</v>
+      </c>
+      <c r="E38" s="3">
+        <f t="shared" si="4"/>
+        <v>57</v>
+      </c>
+      <c r="F38" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="G38" s="3" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="C39" s="3">
+        <v>32.5</v>
+      </c>
+      <c r="D39" s="3">
+        <v>1</v>
+      </c>
+      <c r="E39" s="3">
+        <f t="shared" si="4"/>
+        <v>32.5</v>
+      </c>
+      <c r="F39" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G39" s="3" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="C40" s="3">
+        <v>195</v>
+      </c>
+      <c r="D40" s="3">
+        <v>1</v>
+      </c>
+      <c r="E40" s="3">
+        <f t="shared" si="4"/>
+        <v>195</v>
+      </c>
+      <c r="F40" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G40" s="3" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="C41" s="3">
+        <v>16</v>
+      </c>
+      <c r="D41" s="3">
+        <v>1</v>
+      </c>
+      <c r="E41" s="3">
+        <f t="shared" si="4"/>
+        <v>16</v>
+      </c>
+      <c r="F41" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="G41" s="3" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="C42" s="3">
+        <v>32</v>
+      </c>
+      <c r="D42" s="3">
+        <v>1</v>
+      </c>
+      <c r="E42" s="3">
+        <f t="shared" si="4"/>
+        <v>32</v>
+      </c>
+      <c r="F42" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G42" s="3" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="C43" s="3">
+        <v>19</v>
+      </c>
+      <c r="D43" s="3">
+        <v>1</v>
+      </c>
+      <c r="E43" s="3">
+        <f t="shared" si="4"/>
+        <v>19</v>
+      </c>
+      <c r="F43" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G43" s="3" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="C44" s="3">
+        <v>42</v>
+      </c>
+      <c r="D44" s="3">
+        <v>1</v>
+      </c>
+      <c r="E44" s="3">
+        <f t="shared" si="4"/>
+        <v>42</v>
+      </c>
+      <c r="F44" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G44" s="3" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="C45" s="3">
+        <v>50</v>
+      </c>
+      <c r="D45" s="3">
+        <v>1</v>
+      </c>
+      <c r="E45" s="3">
+        <f t="shared" si="4"/>
+        <v>50</v>
+      </c>
+      <c r="F45" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G45" s="3" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="C46" s="3">
+        <v>42.5</v>
+      </c>
+      <c r="D46" s="3">
+        <v>1</v>
+      </c>
+      <c r="E46" s="3">
+        <f t="shared" si="4"/>
+        <v>42.5</v>
+      </c>
+      <c r="F46" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G46" s="3" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="C47" s="3">
+        <v>10</v>
+      </c>
+      <c r="D47" s="3">
+        <v>1</v>
+      </c>
+      <c r="E47" s="3">
+        <f t="shared" ref="E47" si="5">C47*D47</f>
+        <v>10</v>
+      </c>
+      <c r="F47" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G47" s="3" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="C48" s="3">
+        <v>15</v>
+      </c>
+      <c r="D48" s="3">
+        <v>2</v>
+      </c>
+      <c r="E48" s="3">
+        <f t="shared" ref="E48" si="6">C48*D48</f>
+        <v>30</v>
+      </c>
+      <c r="F48" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G48" s="3" t="s">
+        <v>148</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Git008 -updated November and December month expenses
</commit_message>
<xml_diff>
--- a/TestMonthlyExpense/src/main/resources/HouseExpenseChart.xlsx
+++ b/TestMonthlyExpense/src/main/resources/HouseExpenseChart.xlsx
@@ -4,18 +4,21 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="August" sheetId="2" r:id="rId1"/>
     <sheet name="September" sheetId="3" r:id="rId2"/>
+    <sheet name="October" sheetId="4" r:id="rId3"/>
+    <sheet name="November" sheetId="5" r:id="rId4"/>
+    <sheet name="December" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="442" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="805" uniqueCount="207">
   <si>
     <t>GF</t>
   </si>
@@ -462,6 +465,180 @@
   </si>
   <si>
     <t>September</t>
+  </si>
+  <si>
+    <t>Purchased in local shop</t>
+  </si>
+  <si>
+    <t>November</t>
+  </si>
+  <si>
+    <t>Roasted Rava 500g</t>
+  </si>
+  <si>
+    <t>Raisins 200g</t>
+  </si>
+  <si>
+    <t>Pattai 10g</t>
+  </si>
+  <si>
+    <t>ManjalThool 500g</t>
+  </si>
+  <si>
+    <t>Noodles 420g</t>
+  </si>
+  <si>
+    <t>Dish wash Liquid 1L</t>
+  </si>
+  <si>
+    <t>Harpic rose</t>
+  </si>
+  <si>
+    <t>Harpic orange</t>
+  </si>
+  <si>
+    <t>Tea 250g</t>
+  </si>
+  <si>
+    <t>Annasipoo 25g</t>
+  </si>
+  <si>
+    <t>Jathipathri 10g</t>
+  </si>
+  <si>
+    <t>Popular</t>
+  </si>
+  <si>
+    <t>Appalam mini</t>
+  </si>
+  <si>
+    <t>Bels</t>
+  </si>
+  <si>
+    <t>Noodles veg</t>
+  </si>
+  <si>
+    <t>Samaai rice 500g</t>
+  </si>
+  <si>
+    <t>Cartex</t>
+  </si>
+  <si>
+    <t>Olive oil 500ml</t>
+  </si>
+  <si>
+    <t>GreenLabel</t>
+  </si>
+  <si>
+    <t>Coffee 100g</t>
+  </si>
+  <si>
+    <t>Bru</t>
+  </si>
+  <si>
+    <t>Health drink</t>
+  </si>
+  <si>
+    <t>Tomato sauce</t>
+  </si>
+  <si>
+    <t>Sabeena</t>
+  </si>
+  <si>
+    <t>Washing powder 1kg</t>
+  </si>
+  <si>
+    <t>Rin</t>
+  </si>
+  <si>
+    <t>Inscet killer</t>
+  </si>
+  <si>
+    <t>Parachute</t>
+  </si>
+  <si>
+    <t>Hair oil</t>
+  </si>
+  <si>
+    <t>SS</t>
+  </si>
+  <si>
+    <t>Shampoo</t>
+  </si>
+  <si>
+    <t>RIM</t>
+  </si>
+  <si>
+    <t>Tap Filter</t>
+  </si>
+  <si>
+    <t>Washing bar</t>
+  </si>
+  <si>
+    <t>Axe</t>
+  </si>
+  <si>
+    <t>Oil</t>
+  </si>
+  <si>
+    <t>Dabur</t>
+  </si>
+  <si>
+    <t>Almond Oil</t>
+  </si>
+  <si>
+    <t>Odonil</t>
+  </si>
+  <si>
+    <t>Dustbag Large</t>
+  </si>
+  <si>
+    <t>Dustbag small</t>
+  </si>
+  <si>
+    <t>December</t>
+  </si>
+  <si>
+    <t>Noodles 340g</t>
+  </si>
+  <si>
+    <t>Seeragam 200g</t>
+  </si>
+  <si>
+    <t>Bath Soap 150g</t>
+  </si>
+  <si>
+    <t>Toothpaste 150g</t>
+  </si>
+  <si>
+    <t>Samaai rice 750g</t>
+  </si>
+  <si>
+    <t>Olive oil 1l</t>
+  </si>
+  <si>
+    <t>Tomato sauce 465g</t>
+  </si>
+  <si>
+    <t>Hair oil 250ml</t>
+  </si>
+  <si>
+    <t>Good Night</t>
+  </si>
+  <si>
+    <t>Mosquito killer Liquid</t>
+  </si>
+  <si>
+    <t>Dustbag medium</t>
+  </si>
+  <si>
+    <t>Green Peas 500g</t>
+  </si>
+  <si>
+    <t>Odonil bathroom freshner</t>
+  </si>
+  <si>
+    <t>Brinji leaf / Bay Leaf</t>
   </si>
 </sst>
 </file>
@@ -626,7 +803,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="35">
+  <fills count="37">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -818,6 +995,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="11">
     <border>
@@ -994,12 +1183,14 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="20" fillId="34" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="35" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="36" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1345,7 +1536,7 @@
   <dimension ref="A1:H61"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2818,8 +3009,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3:G48"/>
+    <sheetView topLeftCell="A24" workbookViewId="0">
+      <selection sqref="A1:G48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3987,4 +4178,2205 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>149</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G56"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H46" sqref="H46"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="3">
+        <v>254</v>
+      </c>
+      <c r="D2" s="3">
+        <v>1</v>
+      </c>
+      <c r="E2" s="3">
+        <f>C2*D2</f>
+        <v>254</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="C3" s="3">
+        <v>56</v>
+      </c>
+      <c r="D3" s="3">
+        <v>1</v>
+      </c>
+      <c r="E3" s="3">
+        <f t="shared" ref="E3:E56" si="0">C3*D3</f>
+        <v>56</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="C4" s="3">
+        <v>54.5</v>
+      </c>
+      <c r="D4" s="3">
+        <v>1</v>
+      </c>
+      <c r="E4" s="3">
+        <f t="shared" si="0"/>
+        <v>54.5</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="C5" s="3">
+        <v>105</v>
+      </c>
+      <c r="D5" s="3">
+        <v>1</v>
+      </c>
+      <c r="E5" s="3">
+        <f t="shared" si="0"/>
+        <v>105</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C6" s="3">
+        <v>226</v>
+      </c>
+      <c r="D6" s="3">
+        <v>3</v>
+      </c>
+      <c r="E6" s="3">
+        <f t="shared" si="0"/>
+        <v>678</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="3">
+        <v>66</v>
+      </c>
+      <c r="D7" s="3">
+        <v>1</v>
+      </c>
+      <c r="E7" s="3">
+        <f t="shared" si="0"/>
+        <v>66</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="3">
+        <v>66</v>
+      </c>
+      <c r="D8" s="3">
+        <v>3</v>
+      </c>
+      <c r="E8" s="3">
+        <f t="shared" si="0"/>
+        <v>198</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="3">
+        <v>65</v>
+      </c>
+      <c r="D9" s="3">
+        <v>2</v>
+      </c>
+      <c r="E9" s="3">
+        <f t="shared" si="0"/>
+        <v>130</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="C10" s="3">
+        <v>168</v>
+      </c>
+      <c r="D10" s="3">
+        <v>1</v>
+      </c>
+      <c r="E10" s="3">
+        <f t="shared" si="0"/>
+        <v>168</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" s="3">
+        <v>89</v>
+      </c>
+      <c r="D11" s="3">
+        <v>1</v>
+      </c>
+      <c r="E11" s="3">
+        <f t="shared" si="0"/>
+        <v>89</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C12" s="3">
+        <v>41</v>
+      </c>
+      <c r="D12" s="3">
+        <v>1</v>
+      </c>
+      <c r="E12" s="3">
+        <f t="shared" si="0"/>
+        <v>41</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" s="3">
+        <v>102</v>
+      </c>
+      <c r="D13" s="3">
+        <v>2</v>
+      </c>
+      <c r="E13" s="3">
+        <f t="shared" si="0"/>
+        <v>204</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C14" s="3">
+        <v>18</v>
+      </c>
+      <c r="D14" s="3">
+        <v>2</v>
+      </c>
+      <c r="E14" s="3">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C15" s="3">
+        <v>85</v>
+      </c>
+      <c r="D15" s="3">
+        <v>1</v>
+      </c>
+      <c r="E15" s="3">
+        <f t="shared" si="0"/>
+        <v>85</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="C16" s="3">
+        <v>77</v>
+      </c>
+      <c r="D16" s="3">
+        <v>1</v>
+      </c>
+      <c r="E16" s="3">
+        <f t="shared" si="0"/>
+        <v>77</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="C17" s="3">
+        <v>74.5</v>
+      </c>
+      <c r="D17" s="3">
+        <v>1</v>
+      </c>
+      <c r="E17" s="3">
+        <f t="shared" si="0"/>
+        <v>74.5</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C18" s="3">
+        <v>240.5</v>
+      </c>
+      <c r="D18" s="3">
+        <v>1</v>
+      </c>
+      <c r="E18" s="3">
+        <f t="shared" si="0"/>
+        <v>240.5</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="C19" s="3">
+        <v>78</v>
+      </c>
+      <c r="D19" s="3">
+        <v>1</v>
+      </c>
+      <c r="E19" s="3">
+        <f t="shared" si="0"/>
+        <v>78</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="C20" s="3">
+        <v>46.5</v>
+      </c>
+      <c r="D20" s="3">
+        <v>2</v>
+      </c>
+      <c r="E20" s="3">
+        <f t="shared" si="0"/>
+        <v>93</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="C21" s="3">
+        <v>4</v>
+      </c>
+      <c r="D21" s="3">
+        <v>2</v>
+      </c>
+      <c r="E21" s="3">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G21" s="3" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C22" s="3">
+        <v>132</v>
+      </c>
+      <c r="D22" s="3">
+        <v>1</v>
+      </c>
+      <c r="E22" s="3">
+        <f t="shared" si="0"/>
+        <v>132</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="C23" s="3">
+        <v>150</v>
+      </c>
+      <c r="D23" s="3">
+        <v>1</v>
+      </c>
+      <c r="E23" s="3">
+        <f t="shared" si="0"/>
+        <v>150</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G23" s="3" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C24" s="3">
+        <v>25</v>
+      </c>
+      <c r="D24" s="3">
+        <v>6</v>
+      </c>
+      <c r="E24" s="3">
+        <f t="shared" si="0"/>
+        <v>150</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G24" s="3" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="C25" s="3">
+        <v>60</v>
+      </c>
+      <c r="D25" s="3">
+        <v>1</v>
+      </c>
+      <c r="E25" s="3">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G25" s="3" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="C26" s="3">
+        <v>220</v>
+      </c>
+      <c r="D26" s="3">
+        <v>2</v>
+      </c>
+      <c r="E26" s="3">
+        <f t="shared" si="0"/>
+        <v>440</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G26" s="3" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="C27" s="3">
+        <v>20</v>
+      </c>
+      <c r="D27" s="3">
+        <v>2</v>
+      </c>
+      <c r="E27" s="3">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="F27" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G27" s="3" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="C28" s="3">
+        <v>61</v>
+      </c>
+      <c r="D28" s="3">
+        <v>1</v>
+      </c>
+      <c r="E28" s="3">
+        <f t="shared" si="0"/>
+        <v>61</v>
+      </c>
+      <c r="F28" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="G28" s="3" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="C29" s="3">
+        <v>32.5</v>
+      </c>
+      <c r="D29" s="3">
+        <v>1</v>
+      </c>
+      <c r="E29" s="3">
+        <f t="shared" si="0"/>
+        <v>32.5</v>
+      </c>
+      <c r="F29" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G29" s="3" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="C30" s="3">
+        <v>82</v>
+      </c>
+      <c r="D30" s="3">
+        <v>1</v>
+      </c>
+      <c r="E30" s="3">
+        <f t="shared" si="0"/>
+        <v>82</v>
+      </c>
+      <c r="F30" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G30" s="3" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="C31" s="3">
+        <v>27</v>
+      </c>
+      <c r="D31" s="3">
+        <v>2</v>
+      </c>
+      <c r="E31" s="3">
+        <f t="shared" si="0"/>
+        <v>54</v>
+      </c>
+      <c r="F31" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G31" s="3" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="C32" s="3">
+        <v>42.5</v>
+      </c>
+      <c r="D32" s="3">
+        <v>4</v>
+      </c>
+      <c r="E32" s="3">
+        <f t="shared" si="0"/>
+        <v>170</v>
+      </c>
+      <c r="F32" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G32" s="3" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C33" s="3">
+        <v>17</v>
+      </c>
+      <c r="D33" s="3">
+        <v>4</v>
+      </c>
+      <c r="E33" s="3">
+        <f t="shared" si="0"/>
+        <v>68</v>
+      </c>
+      <c r="F33" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G33" s="3" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="C34" s="3">
+        <v>15</v>
+      </c>
+      <c r="D34" s="3">
+        <v>1</v>
+      </c>
+      <c r="E34" s="3">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="F34" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G34" s="3" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="C35" s="3">
+        <v>25</v>
+      </c>
+      <c r="D35" s="3">
+        <v>1</v>
+      </c>
+      <c r="E35" s="3">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="F35" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G35" s="3" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="C36" s="3">
+        <v>24</v>
+      </c>
+      <c r="D36" s="3">
+        <v>2</v>
+      </c>
+      <c r="E36" s="3">
+        <f t="shared" si="0"/>
+        <v>48</v>
+      </c>
+      <c r="F36" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G36" s="3" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="C37" s="3">
+        <v>25</v>
+      </c>
+      <c r="D37" s="3">
+        <v>2</v>
+      </c>
+      <c r="E37" s="3">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="F37" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G37" s="3" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="C38" s="3">
+        <v>46.5</v>
+      </c>
+      <c r="D38" s="3">
+        <v>1</v>
+      </c>
+      <c r="E38" s="3">
+        <f t="shared" si="0"/>
+        <v>46.5</v>
+      </c>
+      <c r="F38" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="G38" s="3" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="C39" s="3">
+        <v>222</v>
+      </c>
+      <c r="D39" s="3">
+        <v>1</v>
+      </c>
+      <c r="E39" s="3">
+        <f t="shared" si="0"/>
+        <v>222</v>
+      </c>
+      <c r="F39" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G39" s="3" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="C40" s="3">
+        <v>28</v>
+      </c>
+      <c r="D40" s="3">
+        <v>1</v>
+      </c>
+      <c r="E40" s="3">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+      <c r="F40" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G40" s="3" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="C41" s="3">
+        <v>84</v>
+      </c>
+      <c r="D41" s="3">
+        <v>1</v>
+      </c>
+      <c r="E41" s="3">
+        <f t="shared" si="0"/>
+        <v>84</v>
+      </c>
+      <c r="F41" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G41" s="3" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="C42" s="3">
+        <v>253</v>
+      </c>
+      <c r="D42" s="3">
+        <v>1</v>
+      </c>
+      <c r="E42" s="3">
+        <f t="shared" si="0"/>
+        <v>253</v>
+      </c>
+      <c r="F42" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G42" s="3" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="C43" s="3">
+        <v>88</v>
+      </c>
+      <c r="D43" s="3">
+        <v>1</v>
+      </c>
+      <c r="E43" s="3">
+        <f t="shared" si="0"/>
+        <v>88</v>
+      </c>
+      <c r="F43" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G43" s="3" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C44" s="3">
+        <v>16.5</v>
+      </c>
+      <c r="D44" s="3">
+        <v>2</v>
+      </c>
+      <c r="E44" s="3">
+        <f t="shared" si="0"/>
+        <v>33</v>
+      </c>
+      <c r="F44" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G44" s="3" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="C45" s="3">
+        <v>21.5</v>
+      </c>
+      <c r="D45" s="3">
+        <v>2</v>
+      </c>
+      <c r="E45" s="3">
+        <f t="shared" si="0"/>
+        <v>43</v>
+      </c>
+      <c r="F45" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G45" s="3" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="C46" s="3">
+        <v>82</v>
+      </c>
+      <c r="D46" s="3">
+        <v>1</v>
+      </c>
+      <c r="E46" s="3">
+        <f t="shared" si="0"/>
+        <v>82</v>
+      </c>
+      <c r="F46" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G46" s="3" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="C47" s="3">
+        <v>134</v>
+      </c>
+      <c r="D47" s="3">
+        <v>1</v>
+      </c>
+      <c r="E47" s="3">
+        <f t="shared" si="0"/>
+        <v>134</v>
+      </c>
+      <c r="F47" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G47" s="3" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="C48" s="3">
+        <v>85</v>
+      </c>
+      <c r="D48" s="3">
+        <v>2</v>
+      </c>
+      <c r="E48" s="3">
+        <f t="shared" si="0"/>
+        <v>170</v>
+      </c>
+      <c r="F48" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G48" s="3" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A49" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="C49" s="3">
+        <v>122</v>
+      </c>
+      <c r="D49" s="3">
+        <v>1</v>
+      </c>
+      <c r="E49" s="3">
+        <f t="shared" si="0"/>
+        <v>122</v>
+      </c>
+      <c r="F49" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G49" s="3" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A50" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="C50" s="3">
+        <v>27</v>
+      </c>
+      <c r="D50" s="3">
+        <v>1</v>
+      </c>
+      <c r="E50" s="3">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+      <c r="F50" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G50" s="3" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A51" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="B51" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="C51" s="3">
+        <v>9.5</v>
+      </c>
+      <c r="D51" s="3">
+        <v>4</v>
+      </c>
+      <c r="E51" s="3">
+        <f t="shared" si="0"/>
+        <v>38</v>
+      </c>
+      <c r="F51" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G51" s="3" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A52" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="C52" s="3">
+        <v>138</v>
+      </c>
+      <c r="D52" s="3">
+        <v>1</v>
+      </c>
+      <c r="E52" s="3">
+        <f t="shared" si="0"/>
+        <v>138</v>
+      </c>
+      <c r="F52" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G52" s="3" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A53" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="B53" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="C53" s="3">
+        <v>57</v>
+      </c>
+      <c r="D53" s="3">
+        <v>1</v>
+      </c>
+      <c r="E53" s="3">
+        <f t="shared" si="0"/>
+        <v>57</v>
+      </c>
+      <c r="F53" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G53" s="3" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A54" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C54" s="3">
+        <v>51.5</v>
+      </c>
+      <c r="D54" s="3">
+        <v>1</v>
+      </c>
+      <c r="E54" s="3">
+        <f t="shared" si="0"/>
+        <v>51.5</v>
+      </c>
+      <c r="F54" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G54" s="3" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A55" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B55" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="C55" s="3">
+        <v>84</v>
+      </c>
+      <c r="D55" s="3">
+        <v>2</v>
+      </c>
+      <c r="E55" s="3">
+        <f t="shared" si="0"/>
+        <v>168</v>
+      </c>
+      <c r="F55" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G55" s="3" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A56" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B56" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="C56" s="3">
+        <v>44</v>
+      </c>
+      <c r="D56" s="3">
+        <v>1</v>
+      </c>
+      <c r="E56" s="3">
+        <f t="shared" si="0"/>
+        <v>44</v>
+      </c>
+      <c r="F56" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G56" s="3" t="s">
+        <v>150</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G33"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection sqref="A1:G33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="5">
+        <v>257</v>
+      </c>
+      <c r="D2" s="5">
+        <v>3</v>
+      </c>
+      <c r="E2" s="5">
+        <f>C2*D2</f>
+        <v>771</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="C3" s="5">
+        <v>95</v>
+      </c>
+      <c r="D3" s="5">
+        <v>2</v>
+      </c>
+      <c r="E3" s="5">
+        <f t="shared" ref="E3:E33" si="0">C3*D3</f>
+        <v>190</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="5">
+        <v>32.5</v>
+      </c>
+      <c r="D4" s="5">
+        <v>2</v>
+      </c>
+      <c r="E4" s="5">
+        <f t="shared" si="0"/>
+        <v>65</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="5">
+        <v>130</v>
+      </c>
+      <c r="D5" s="5">
+        <v>1</v>
+      </c>
+      <c r="E5" s="5">
+        <f t="shared" si="0"/>
+        <v>130</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="C6" s="5">
+        <v>120</v>
+      </c>
+      <c r="D6" s="5">
+        <v>3</v>
+      </c>
+      <c r="E6" s="5">
+        <f t="shared" si="0"/>
+        <v>360</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="C7" s="5">
+        <v>172</v>
+      </c>
+      <c r="D7" s="5">
+        <v>1</v>
+      </c>
+      <c r="E7" s="5">
+        <f t="shared" si="0"/>
+        <v>172</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" s="5">
+        <v>88</v>
+      </c>
+      <c r="D8" s="5">
+        <v>1</v>
+      </c>
+      <c r="E8" s="5">
+        <f t="shared" si="0"/>
+        <v>88</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9" s="5">
+        <v>55</v>
+      </c>
+      <c r="D9" s="5">
+        <v>1</v>
+      </c>
+      <c r="E9" s="5">
+        <f t="shared" si="0"/>
+        <v>55</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="C10" s="5">
+        <v>59</v>
+      </c>
+      <c r="D10" s="5">
+        <v>1</v>
+      </c>
+      <c r="E10" s="5">
+        <f t="shared" si="0"/>
+        <v>59</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C11" s="5">
+        <v>105</v>
+      </c>
+      <c r="D11" s="5">
+        <v>1</v>
+      </c>
+      <c r="E11" s="5">
+        <f t="shared" si="0"/>
+        <v>105</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C12" s="5">
+        <v>55</v>
+      </c>
+      <c r="D12" s="5">
+        <v>1</v>
+      </c>
+      <c r="E12" s="5">
+        <f t="shared" si="0"/>
+        <v>55</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C13" s="5">
+        <v>252</v>
+      </c>
+      <c r="D13" s="5">
+        <v>1</v>
+      </c>
+      <c r="E13" s="5">
+        <f t="shared" si="0"/>
+        <v>252</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C14" s="5">
+        <v>85</v>
+      </c>
+      <c r="D14" s="5">
+        <v>1</v>
+      </c>
+      <c r="E14" s="5">
+        <f t="shared" si="0"/>
+        <v>85</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G14" s="5" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="C15" s="5">
+        <v>155</v>
+      </c>
+      <c r="D15" s="5">
+        <v>1</v>
+      </c>
+      <c r="E15" s="5">
+        <f t="shared" si="0"/>
+        <v>155</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G15" s="5" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>195</v>
+      </c>
+      <c r="C16" s="5">
+        <v>38</v>
+      </c>
+      <c r="D16" s="5">
+        <v>6</v>
+      </c>
+      <c r="E16" s="5">
+        <f t="shared" si="0"/>
+        <v>228</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G16" s="5" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="C17" s="5">
+        <v>220</v>
+      </c>
+      <c r="D17" s="5">
+        <v>2</v>
+      </c>
+      <c r="E17" s="5">
+        <f t="shared" si="0"/>
+        <v>440</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G17" s="5" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="C18" s="5">
+        <v>84</v>
+      </c>
+      <c r="D18" s="5">
+        <v>3</v>
+      </c>
+      <c r="E18" s="5">
+        <f t="shared" si="0"/>
+        <v>252</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G18" s="5" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C19" s="5">
+        <v>17.5</v>
+      </c>
+      <c r="D19" s="5">
+        <v>3</v>
+      </c>
+      <c r="E19" s="5">
+        <f t="shared" si="0"/>
+        <v>52.5</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="G19" s="5" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="C20" s="5">
+        <v>59</v>
+      </c>
+      <c r="D20" s="5">
+        <v>1</v>
+      </c>
+      <c r="E20" s="5">
+        <f t="shared" si="0"/>
+        <v>59</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G20" s="5" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>197</v>
+      </c>
+      <c r="C21" s="5">
+        <v>109</v>
+      </c>
+      <c r="D21" s="5">
+        <v>1</v>
+      </c>
+      <c r="E21" s="5">
+        <f t="shared" si="0"/>
+        <v>109</v>
+      </c>
+      <c r="F21" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="G21" s="5" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="C22" s="5">
+        <v>495</v>
+      </c>
+      <c r="D22" s="5">
+        <v>1</v>
+      </c>
+      <c r="E22" s="5">
+        <f t="shared" si="0"/>
+        <v>495</v>
+      </c>
+      <c r="F22" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="G22" s="5" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="C23" s="5">
+        <v>174</v>
+      </c>
+      <c r="D23" s="5">
+        <v>1</v>
+      </c>
+      <c r="E23" s="5">
+        <f t="shared" si="0"/>
+        <v>174</v>
+      </c>
+      <c r="F23" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="G23" s="5" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="C24" s="5">
+        <v>253</v>
+      </c>
+      <c r="D24" s="5">
+        <v>1</v>
+      </c>
+      <c r="E24" s="5">
+        <f t="shared" si="0"/>
+        <v>253</v>
+      </c>
+      <c r="F24" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="G24" s="5" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>199</v>
+      </c>
+      <c r="C25" s="5">
+        <v>95</v>
+      </c>
+      <c r="D25" s="5">
+        <v>1</v>
+      </c>
+      <c r="E25" s="5">
+        <f t="shared" si="0"/>
+        <v>95</v>
+      </c>
+      <c r="F25" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="G25" s="5" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C26" s="5">
+        <v>17</v>
+      </c>
+      <c r="D26" s="5">
+        <v>2</v>
+      </c>
+      <c r="E26" s="5">
+        <f t="shared" si="0"/>
+        <v>34</v>
+      </c>
+      <c r="F26" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="G26" s="5" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="C27" s="5">
+        <v>86</v>
+      </c>
+      <c r="D27" s="5">
+        <v>1</v>
+      </c>
+      <c r="E27" s="5">
+        <f t="shared" si="0"/>
+        <v>86</v>
+      </c>
+      <c r="F27" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G27" s="5" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="C28" s="5">
+        <v>87</v>
+      </c>
+      <c r="D28" s="5">
+        <v>3</v>
+      </c>
+      <c r="E28" s="5">
+        <f t="shared" si="0"/>
+        <v>261</v>
+      </c>
+      <c r="F28" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G28" s="5" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="5" t="s">
+        <v>201</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="C29" s="5">
+        <v>66</v>
+      </c>
+      <c r="D29" s="5">
+        <v>4</v>
+      </c>
+      <c r="E29" s="5">
+        <f t="shared" si="0"/>
+        <v>264</v>
+      </c>
+      <c r="F29" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G29" s="5" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B30" s="6" t="s">
+        <v>203</v>
+      </c>
+      <c r="C30" s="6">
+        <v>75</v>
+      </c>
+      <c r="D30" s="6">
+        <v>1</v>
+      </c>
+      <c r="E30" s="6">
+        <f t="shared" si="0"/>
+        <v>75</v>
+      </c>
+      <c r="F30" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G30" s="6" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B31" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="C31" s="6">
+        <v>59</v>
+      </c>
+      <c r="D31" s="6">
+        <v>1</v>
+      </c>
+      <c r="E31" s="6">
+        <f t="shared" si="0"/>
+        <v>59</v>
+      </c>
+      <c r="F31" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G31" s="6" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B32" s="6" t="s">
+        <v>205</v>
+      </c>
+      <c r="C32" s="6">
+        <v>37</v>
+      </c>
+      <c r="D32" s="6">
+        <v>4</v>
+      </c>
+      <c r="E32" s="6">
+        <f t="shared" si="0"/>
+        <v>148</v>
+      </c>
+      <c r="F32" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G32" s="6" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B33" s="6" t="s">
+        <v>206</v>
+      </c>
+      <c r="C33" s="6">
+        <v>14</v>
+      </c>
+      <c r="D33" s="6">
+        <v>1</v>
+      </c>
+      <c r="E33" s="6">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="F33" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G33" s="6" t="s">
+        <v>192</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>